<commit_message>
Udated model fitting to include estimation of "lambda" parameters, dive success rate (by prey type, group, and all)
</commit_message>
<xml_diff>
--- a/preylib/Energy.xlsx
+++ b/preylib/Energy.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/preylib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_8682FCB9C83D7B0B554A1651FDEE013948FAF44C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AA14E784-91CA-468C-AED2-0C3AA670F835}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_8682FCB9C83D7B0B554A1651FDEE013948FAF44C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{81A35345-A538-4E85-A976-E0ADC6247A49}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="24150" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="165" windowWidth="28095" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Energy!$A$1:$AH$394</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Energy!$A$1:$AH$395</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -595,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -631,6 +631,7 @@
     <xf numFmtId="2" fontId="9" fillId="9" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,10 +971,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AH395"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C394" sqref="C394"/>
+      <selection activeCell="R296" sqref="R296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +986,7 @@
     <col min="9" max="9" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="20.7109375" customWidth="1"/>
     <col min="15" max="15" width="18.5703125" customWidth="1"/>
@@ -1112,7 +1114,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1153,7 +1155,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1194,7 +1196,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1235,7 +1237,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1276,7 +1278,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1358,7 +1360,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1399,7 +1401,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1475,7 +1477,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1516,7 +1518,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1551,7 +1553,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1586,7 +1588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1621,7 +1623,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1662,7 +1664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1703,7 +1705,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1744,7 +1746,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1785,7 +1787,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1826,7 +1828,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1867,7 +1869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1902,7 +1904,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1943,7 +1945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1984,7 +1986,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2025,7 +2027,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2066,7 +2068,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2107,7 +2109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2148,7 +2150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2230,7 +2232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2271,7 +2273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2312,7 +2314,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2347,7 +2349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2382,7 +2384,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2423,7 +2425,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2458,7 +2460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2493,7 +2495,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2528,7 +2530,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2569,7 +2571,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2651,7 +2653,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2692,7 +2694,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2733,7 +2735,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2774,7 +2776,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2815,7 +2817,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2856,7 +2858,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2891,7 +2893,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2932,7 +2934,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2964,7 +2966,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3005,7 +3007,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3046,7 +3048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3078,7 +3080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3119,7 +3121,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3160,7 +3162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -3192,7 +3194,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -3233,7 +3235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -3274,7 +3276,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -3315,7 +3317,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3356,7 +3358,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3438,7 +3440,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -3479,7 +3481,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3514,7 +3516,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -3549,7 +3551,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -3590,7 +3592,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -3631,7 +3633,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -3672,7 +3674,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -3713,7 +3715,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -3754,7 +3756,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -3795,7 +3797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -3836,7 +3838,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -3877,7 +3879,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -3918,7 +3920,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -3959,7 +3961,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -4000,7 +4002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -4041,7 +4043,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -4082,7 +4084,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -4123,7 +4125,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -4164,7 +4166,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -4199,7 +4201,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -4240,7 +4242,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -4281,7 +4283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -4322,7 +4324,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -4363,7 +4365,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -4404,7 +4406,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -4445,7 +4447,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -4486,7 +4488,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -4527,7 +4529,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -4568,7 +4570,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -4609,7 +4611,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -4650,7 +4652,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -4691,7 +4693,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -4732,7 +4734,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -4767,7 +4769,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -4802,7 +4804,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -4843,7 +4845,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -4878,7 +4880,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -4919,7 +4921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -4960,7 +4962,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -4995,7 +4997,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -5036,7 +5038,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5071,7 +5073,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -5103,7 +5105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -5144,7 +5146,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -5179,7 +5181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -5220,7 +5222,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -5252,7 +5254,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -5293,7 +5295,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -5325,7 +5327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -5366,7 +5368,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -5407,7 +5409,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -5448,7 +5450,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -5489,7 +5491,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -5530,7 +5532,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -5571,7 +5573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -5612,7 +5614,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -5647,7 +5649,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -5688,7 +5690,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -5729,7 +5731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -5770,7 +5772,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -5811,7 +5813,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -5852,7 +5854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -5893,7 +5895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -5934,7 +5936,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -5975,7 +5977,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -6016,7 +6018,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -6057,7 +6059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -6098,7 +6100,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -6139,7 +6141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -6180,7 +6182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -6221,7 +6223,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -6262,7 +6264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="132" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -6303,7 +6305,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="133" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -6344,7 +6346,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -6385,7 +6387,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -6426,7 +6428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="136" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -6467,7 +6469,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -6508,7 +6510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -6543,7 +6545,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -6584,7 +6586,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="140" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>139</v>
       </c>
@@ -6625,7 +6627,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="141" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -6666,7 +6668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="142" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>141</v>
       </c>
@@ -6707,7 +6709,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="143" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -6748,7 +6750,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="144" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -6789,7 +6791,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="145" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -6830,7 +6832,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="146" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -6871,7 +6873,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="147" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -6912,7 +6914,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="148" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -6953,7 +6955,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="149" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -6994,7 +6996,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="150" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>149</v>
       </c>
@@ -7035,7 +7037,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="151" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -7076,7 +7078,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="152" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -7117,7 +7119,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="153" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -7149,7 +7151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="154" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -7190,7 +7192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="155" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -7222,7 +7224,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="156" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -7257,7 +7259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="157" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>156</v>
       </c>
@@ -7298,7 +7300,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="158" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -7339,7 +7341,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="159" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -7374,7 +7376,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="160" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -7409,7 +7411,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="161" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -7441,7 +7443,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="162" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -7482,7 +7484,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="163" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -7523,7 +7525,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="164" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -7564,7 +7566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="165" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -7605,7 +7607,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="166" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -7646,7 +7648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="167" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -7687,7 +7689,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="168" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -7728,7 +7730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="169" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -7769,7 +7771,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="170" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -7810,7 +7812,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="171" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -7851,7 +7853,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="172" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -7892,7 +7894,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="173" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -7933,7 +7935,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="174" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -7968,7 +7970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="175" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>174</v>
       </c>
@@ -8009,7 +8011,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="176" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -8044,7 +8046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="177" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -8079,7 +8081,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="178" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -8114,7 +8116,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="179" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -8149,7 +8151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="180" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>179</v>
       </c>
@@ -8190,7 +8192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="181" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>180</v>
       </c>
@@ -8225,7 +8227,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="182" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -8266,7 +8268,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="183" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -8301,7 +8303,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="184" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>183</v>
       </c>
@@ -8342,7 +8344,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="185" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -8374,7 +8376,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="186" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -8409,7 +8411,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="187" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -8444,7 +8446,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="188" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>187</v>
       </c>
@@ -8476,7 +8478,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="189" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -8517,7 +8519,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="190" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -8558,7 +8560,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="191" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -8599,7 +8601,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="192" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -8634,7 +8636,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="193" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -8666,7 +8668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="194" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -8698,7 +8700,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="195" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -8733,7 +8735,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="196" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -8765,7 +8767,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="197" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -8806,7 +8808,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="198" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -8847,7 +8849,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="199" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -8888,7 +8890,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="200" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -8929,7 +8931,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="201" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -8961,7 +8963,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="202" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -8993,7 +8995,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="203" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -9034,7 +9036,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="204" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -9075,7 +9077,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="205" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -9107,7 +9109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="206" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -9148,7 +9150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="207" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>206</v>
       </c>
@@ -9183,7 +9185,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="208" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>207</v>
       </c>
@@ -9224,7 +9226,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="209" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -9265,7 +9267,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="210" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -9306,7 +9308,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="211" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -9347,7 +9349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="212" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -9388,7 +9390,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="213" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -9423,7 +9425,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="214" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -9464,7 +9466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="215" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -9499,7 +9501,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="216" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -9534,7 +9536,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="217" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -9569,7 +9571,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="218" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -9610,7 +9612,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="219" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -9645,7 +9647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="220" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>219</v>
       </c>
@@ -9686,7 +9688,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="221" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -9718,7 +9720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="222" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -9759,7 +9761,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="223" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -9794,7 +9796,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="224" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -9829,7 +9831,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="225" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -9870,7 +9872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="226" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>225</v>
       </c>
@@ -9905,7 +9907,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="227" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>226</v>
       </c>
@@ -9940,7 +9942,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="228" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>227</v>
       </c>
@@ -9975,7 +9977,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="229" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -10007,7 +10009,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="230" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>229</v>
       </c>
@@ -10042,7 +10044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="231" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -10083,7 +10085,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="232" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>231</v>
       </c>
@@ -10118,7 +10120,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="233" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>232</v>
       </c>
@@ -10159,7 +10161,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="234" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>233</v>
       </c>
@@ -10191,7 +10193,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="235" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -10232,7 +10234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="236" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -10273,7 +10275,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="237" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -10308,7 +10310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="238" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -10340,7 +10342,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="239" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>238</v>
       </c>
@@ -10381,7 +10383,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="240" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -10422,7 +10424,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="241" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>240</v>
       </c>
@@ -10463,7 +10465,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="242" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>241</v>
       </c>
@@ -10504,7 +10506,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="243" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -10545,7 +10547,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="244" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -10586,7 +10588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="245" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>244</v>
       </c>
@@ -10627,7 +10629,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="246" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>245</v>
       </c>
@@ -10668,7 +10670,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="247" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>246</v>
       </c>
@@ -10709,7 +10711,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="248" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>247</v>
       </c>
@@ -10750,7 +10752,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="249" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>248</v>
       </c>
@@ -10785,7 +10787,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="250" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -10820,7 +10822,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="251" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -10861,7 +10863,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="252" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>251</v>
       </c>
@@ -10902,7 +10904,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="253" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -10943,7 +10945,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="254" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -10984,7 +10986,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="255" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>254</v>
       </c>
@@ -11025,7 +11027,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="256" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>255</v>
       </c>
@@ -11066,7 +11068,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="257" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>256</v>
       </c>
@@ -11107,7 +11109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="258" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
         <v>257</v>
       </c>
@@ -11148,7 +11150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="259" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
         <v>258</v>
       </c>
@@ -11189,7 +11191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="260" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
         <v>259</v>
       </c>
@@ -11230,7 +11232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="261" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -11271,7 +11273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="262" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -11312,7 +11314,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="263" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -11344,7 +11346,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="264" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -11379,7 +11381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="265" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -11411,7 +11413,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="266" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
         <v>265</v>
       </c>
@@ -11452,7 +11454,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="267" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
         <v>266</v>
       </c>
@@ -11487,7 +11489,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="268" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
         <v>267</v>
       </c>
@@ -11559,6 +11561,7 @@
       <c r="R269" s="7">
         <v>0.31833570272594602</v>
       </c>
+      <c r="S269" s="13"/>
       <c r="U269" s="7">
         <v>3.0029454365270198</v>
       </c>
@@ -12983,7 +12986,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="308" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
         <v>307</v>
       </c>
@@ -13024,7 +13027,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="309" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
         <v>308</v>
       </c>
@@ -13065,7 +13068,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="310" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
         <v>309</v>
       </c>
@@ -13097,7 +13100,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="311" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
         <v>310</v>
       </c>
@@ -13138,7 +13141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="312" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2">
         <v>311</v>
       </c>
@@ -13179,7 +13182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="313" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2">
         <v>312</v>
       </c>
@@ -13220,7 +13223,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="314" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2">
         <v>313</v>
       </c>
@@ -13261,7 +13264,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="315" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="2">
         <v>314</v>
       </c>
@@ -13302,7 +13305,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="316" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2">
         <v>315</v>
       </c>
@@ -13343,7 +13346,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="317" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="2">
         <v>316</v>
       </c>
@@ -13384,7 +13387,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="318" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <v>317</v>
       </c>
@@ -13425,7 +13428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="319" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <v>318</v>
       </c>
@@ -13466,7 +13469,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="320" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2">
         <v>319</v>
       </c>
@@ -13507,7 +13510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="321" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2">
         <v>320</v>
       </c>
@@ -13542,7 +13545,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="322" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2">
         <v>321</v>
       </c>
@@ -13574,7 +13577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="323" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="2">
         <v>322</v>
       </c>
@@ -13615,7 +13618,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="324" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2">
         <v>323</v>
       </c>
@@ -13656,7 +13659,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="325" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2">
         <v>324</v>
       </c>
@@ -13697,7 +13700,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="326" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2">
         <v>325</v>
       </c>
@@ -13738,7 +13741,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="327" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2">
         <v>326</v>
       </c>
@@ -13773,7 +13776,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="328" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2">
         <v>327</v>
       </c>
@@ -13808,7 +13811,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="329" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2">
         <v>328</v>
       </c>
@@ -13843,7 +13846,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="330" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2">
         <v>329</v>
       </c>
@@ -13884,7 +13887,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="331" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2">
         <v>330</v>
       </c>
@@ -13925,7 +13928,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="332" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="2">
         <v>331</v>
       </c>
@@ -13966,7 +13969,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="333" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="2">
         <v>332</v>
       </c>
@@ -14007,7 +14010,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="334" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="2">
         <v>333</v>
       </c>
@@ -14048,7 +14051,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="335" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="2">
         <v>334</v>
       </c>
@@ -14089,7 +14092,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="336" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="2">
         <v>335</v>
       </c>
@@ -14130,7 +14133,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="337" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2">
         <v>336</v>
       </c>
@@ -14171,7 +14174,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="338" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2">
         <v>337</v>
       </c>
@@ -14212,7 +14215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="339" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="2">
         <v>338</v>
       </c>
@@ -14247,7 +14250,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="340" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <v>339</v>
       </c>
@@ -14288,7 +14291,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="341" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="2">
         <v>340</v>
       </c>
@@ -14329,7 +14332,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="342" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2">
         <v>341</v>
       </c>
@@ -14370,7 +14373,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="343" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="2">
         <v>342</v>
       </c>
@@ -14405,7 +14408,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="344" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2">
         <v>343</v>
       </c>
@@ -14440,7 +14443,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="345" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2">
         <v>344</v>
       </c>
@@ -14475,7 +14478,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="346" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2">
         <v>345</v>
       </c>
@@ -14510,7 +14513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="347" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="2">
         <v>346</v>
       </c>
@@ -14551,7 +14554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="348" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2">
         <v>347</v>
       </c>
@@ -14592,7 +14595,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="349" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="2">
         <v>348</v>
       </c>
@@ -14633,7 +14636,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="350" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
         <v>349</v>
       </c>
@@ -14674,7 +14677,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="351" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
         <v>350</v>
       </c>
@@ -14715,7 +14718,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="352" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2">
         <v>351</v>
       </c>
@@ -14750,7 +14753,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="353" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="2">
         <v>352</v>
       </c>
@@ -14785,7 +14788,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="354" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="2">
         <v>353</v>
       </c>
@@ -14826,7 +14829,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="355" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="2">
         <v>354</v>
       </c>
@@ -14867,7 +14870,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="356" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2">
         <v>356</v>
       </c>
@@ -14914,7 +14917,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="357" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2">
         <v>357</v>
       </c>
@@ -14961,7 +14964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="358" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2">
         <v>358</v>
       </c>
@@ -15008,7 +15011,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="359" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2">
         <v>359</v>
       </c>
@@ -15055,7 +15058,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="360" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <v>360</v>
       </c>
@@ -15102,7 +15105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="361" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <v>361</v>
       </c>
@@ -15149,7 +15152,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="362" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <v>362</v>
       </c>
@@ -15196,7 +15199,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="363" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2">
         <v>363</v>
       </c>
@@ -15243,7 +15246,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="364" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2">
         <v>364</v>
       </c>
@@ -15290,7 +15293,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="365" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2">
         <v>365</v>
       </c>
@@ -15337,7 +15340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="366" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="2">
         <v>366</v>
       </c>
@@ -15384,7 +15387,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="367" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2">
         <v>367</v>
       </c>
@@ -15431,7 +15434,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="368" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2">
         <v>368</v>
       </c>
@@ -15478,7 +15481,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="369" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="2">
         <v>369</v>
       </c>
@@ -15525,7 +15528,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="370" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="2">
         <v>370</v>
       </c>
@@ -15572,7 +15575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="371" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="2">
         <v>371</v>
       </c>
@@ -15619,7 +15622,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="372" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2">
         <v>372</v>
       </c>
@@ -15666,7 +15669,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="373" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="2">
         <v>373</v>
       </c>
@@ -15713,7 +15716,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="374" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2">
         <v>374</v>
       </c>
@@ -15760,7 +15763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="375" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2">
         <v>375</v>
       </c>
@@ -15807,7 +15810,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="376" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2">
         <v>376</v>
       </c>
@@ -15854,7 +15857,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="377" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="2">
         <v>377</v>
       </c>
@@ -15901,7 +15904,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="378" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="2">
         <v>378</v>
       </c>
@@ -15948,7 +15951,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="379" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="2">
         <v>379</v>
       </c>
@@ -15995,7 +15998,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="380" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="2">
         <v>380</v>
       </c>
@@ -16042,7 +16045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="381" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="2">
         <v>381</v>
       </c>
@@ -16089,7 +16092,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="382" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2">
         <v>382</v>
       </c>
@@ -16136,7 +16139,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="383" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="2">
         <v>383</v>
       </c>
@@ -16183,7 +16186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="384" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="2">
         <v>384</v>
       </c>
@@ -16230,7 +16233,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="385" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="2">
         <v>385</v>
       </c>
@@ -16277,7 +16280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="386" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="2">
         <v>386</v>
       </c>
@@ -16324,7 +16327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="387" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2">
         <v>387</v>
       </c>
@@ -16371,7 +16374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="388" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="2">
         <v>388</v>
       </c>
@@ -16462,7 +16465,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="390" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="2">
         <v>390</v>
       </c>
@@ -16497,7 +16500,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="391" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="2">
         <v>391</v>
       </c>
@@ -16532,7 +16535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="392" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="2">
         <v>392</v>
       </c>
@@ -16579,7 +16582,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="393" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="2">
         <v>393</v>
       </c>
@@ -16626,7 +16629,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="394" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:34" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="2">
         <v>394</v>
       </c>
@@ -16670,7 +16673,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="395" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="9">
         <v>395</v>
       </c>
@@ -16739,7 +16742,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH394" xr:uid="{775E4862-0FF5-45F4-8733-3DBF4FEDE70D}"/>
+  <autoFilter ref="A1:AH395" xr:uid="{775E4862-0FF5-45F4-8733-3DBF4FEDE70D}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="STFR"/>
+        <filter val="STPU"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update SOFA to version 3 (major update)
</commit_message>
<xml_diff>
--- a/preylib/Energy.xlsx
+++ b/preylib/Energy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhydra-my.sharepoint.com/personal/ttinker_nhydra-eco_com/Documents/SOFA2/SOFA/preylib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{4395BD3F-6ED6-4086-96BC-F81FF3DCEE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8BE72B1-56EE-4E78-9277-CEDBFADC6324}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{4395BD3F-6ED6-4086-96BC-F81FF3DCEE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC80D7B3-49BD-42E7-9C36-93AF4D5B4390}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4290" yWindow="1530" windowWidth="41940" windowHeight="20070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="1200" windowWidth="37320" windowHeight="18315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy_NLL" sheetId="1" r:id="rId1"/>
@@ -4037,6 +4037,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -4337,9 +4341,9 @@
   <dimension ref="A1:BE914"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A543" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A438" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S545" sqref="S545"/>
+      <selection pane="bottomLeft" activeCell="S916" sqref="S916"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>